<commit_message>
refactor name of attributes in cycle z
</commit_message>
<xml_diff>
--- a/Data/Chickens data/DataCycleCleaning.xlsx
+++ b/Data/Chickens data/DataCycleCleaning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\Documents\DASA---Project\Data\Chickens data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C62019-7EAA-4C15-9197-EF54F0E25884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC6A924-B7D8-4A4E-8890-14FB45992446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="20">
   <si>
     <t>0</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>Laied</t>
-  </si>
-  <si>
-    <t>42139</t>
   </si>
 </sst>
 </file>
@@ -540,11 +537,11 @@
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0F10D011-4763-4501-88FD-E8AEF2A6CCBA}" name="Arrival Chickens Date" totalsRowLabel="Total" dataDxfId="32" totalsRowDxfId="31"/>
     <tableColumn id="2" xr3:uid="{0C8A19F1-F4A0-4F0B-9886-086176DAF095}" name="Death" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{2DA2A574-E6E5-461A-8F31-DAD7F9FCDADF}" name="42139" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{2DA2A574-E6E5-461A-8F31-DAD7F9FCDADF}" name="Chickens" dataDxfId="28" totalsRowDxfId="27"/>
     <tableColumn id="4" xr3:uid="{27B76BE9-CA3C-4828-9E09-307D98140C5E}" name="Date of Laid" dataDxfId="26" totalsRowDxfId="25"/>
     <tableColumn id="5" xr3:uid="{1A06C482-F450-40C7-A151-18E79B0959F7}" name="Eggs" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
     <tableColumn id="6" xr3:uid="{C9133909-0F95-40AE-9EEB-B2129C58AB9B}" name="Laied" dataDxfId="22" totalsRowDxfId="21">
-      <calculatedColumnFormula>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</calculatedColumnFormula>
+      <calculatedColumnFormula>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{21FAD57B-C2B1-4218-ABA8-6A88CB2AFB5B}" name="Water" dataDxfId="20" totalsRowDxfId="19"/>
     <tableColumn id="8" xr3:uid="{EE8EE056-0125-4426-B0A8-B73C0D71CBF3}" name="Feed" dataDxfId="18" totalsRowDxfId="17"/>
@@ -8093,7 +8090,7 @@
   <dimension ref="A1:K509"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8119,7 +8116,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -8163,7 +8160,7 @@
         <v>30080</v>
       </c>
       <c r="F2">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71398053643484449</v>
       </c>
       <c r="G2" s="6"/>
@@ -8194,7 +8191,7 @@
         <v>31710</v>
       </c>
       <c r="F3">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75283112936539964</v>
       </c>
       <c r="G3" s="6"/>
@@ -8225,7 +8222,7 @@
         <v>33800</v>
       </c>
       <c r="F4">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80269782464139827</v>
       </c>
       <c r="G4" s="6"/>
@@ -8256,7 +8253,7 @@
         <v>34330</v>
       </c>
       <c r="F5">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81547816998432232</v>
       </c>
       <c r="G5" s="6"/>
@@ -8287,7 +8284,7 @@
         <v>34050</v>
       </c>
       <c r="F6">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80905764387207146</v>
       </c>
       <c r="G6" s="6"/>
@@ -8318,7 +8315,7 @@
         <v>37110</v>
       </c>
       <c r="F7">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88195451196615726</v>
       </c>
       <c r="G7" s="6"/>
@@ -8349,7 +8346,7 @@
         <v>37050</v>
       </c>
       <c r="F8">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88080068467097761</v>
       </c>
       <c r="G8" s="6"/>
@@ -8380,7 +8377,7 @@
         <v>36550</v>
       </c>
       <c r="F9">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86914132166551727</v>
       </c>
       <c r="G9" s="6"/>
@@ -8411,7 +8408,7 @@
         <v>37290</v>
       </c>
       <c r="F10">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88688579175189075</v>
       </c>
       <c r="G10" s="6"/>
@@ -8442,7 +8439,7 @@
         <v>37980</v>
       </c>
       <c r="F11">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90348978281038128</v>
       </c>
       <c r="G11" s="6"/>
@@ -8473,7 +8470,7 @@
         <v>36700</v>
       </c>
       <c r="F12">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87324814999881029</v>
       </c>
       <c r="G12" s="6"/>
@@ -8504,7 +8501,7 @@
         <v>38970</v>
       </c>
       <c r="F13">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92743758775791907</v>
       </c>
       <c r="G13" s="6"/>
@@ -8535,7 +8532,7 @@
         <v>38890</v>
       </c>
       <c r="F14">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92570993311275618</v>
       </c>
       <c r="G14" s="6"/>
@@ -8566,7 +8563,7 @@
         <v>37120</v>
       </c>
       <c r="F15">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88376743964573112</v>
       </c>
       <c r="G15" s="6"/>
@@ -8597,7 +8594,7 @@
         <v>40440</v>
       </c>
       <c r="F16">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9629259232802343</v>
       </c>
       <c r="G16" s="6"/>
@@ -8628,7 +8625,7 @@
         <v>40260</v>
       </c>
       <c r="F17">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95879971421767085</v>
       </c>
       <c r="G17" s="6"/>
@@ -8659,7 +8656,7 @@
         <v>38810</v>
       </c>
       <c r="F18">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92437775395974753</v>
       </c>
       <c r="G18" s="6"/>
@@ -8690,7 +8687,7 @@
         <v>40340</v>
       </c>
       <c r="F19">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96091088825897431</v>
       </c>
       <c r="G19" s="6"/>
@@ -8721,7 +8718,7 @@
         <v>39520</v>
       </c>
       <c r="F20">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94164740641902356</v>
       </c>
       <c r="G20" s="6"/>
@@ -8752,7 +8749,7 @@
         <v>38930</v>
       </c>
       <c r="F21">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9277220408455068</v>
       </c>
       <c r="G21" s="6"/>
@@ -8783,7 +8780,7 @@
         <v>39200</v>
       </c>
       <c r="F22">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93442349407642245</v>
       </c>
       <c r="G22" s="6"/>
@@ -8814,7 +8811,7 @@
         <v>39180</v>
       </c>
       <c r="F23">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93405807466742952</v>
       </c>
       <c r="G23" s="6"/>
@@ -8845,7 +8842,7 @@
         <v>39790</v>
       </c>
       <c r="F24">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94889466529940625</v>
       </c>
       <c r="G24" s="6"/>
@@ -8876,7 +8873,7 @@
         <v>40520</v>
       </c>
       <c r="F25">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96641862240030529</v>
       </c>
       <c r="G25" s="6"/>
@@ -8907,7 +8904,7 @@
         <v>39880</v>
       </c>
       <c r="F26">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95126780049137705</v>
       </c>
       <c r="G26" s="6"/>
@@ -8938,7 +8935,7 @@
         <v>39090</v>
       </c>
       <c r="F27">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93262394426683204</v>
       </c>
       <c r="G27" s="6"/>
@@ -8969,7 +8966,7 @@
         <v>39300</v>
       </c>
       <c r="F28">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9379251091859383</v>
       </c>
       <c r="G28" s="6"/>
@@ -9000,7 +8997,7 @@
         <v>40150</v>
       </c>
       <c r="F29">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9583482515813343</v>
       </c>
       <c r="G29" s="6"/>
@@ -9031,7 +9028,7 @@
         <v>39750</v>
       </c>
       <c r="F30">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9489138219145381</v>
       </c>
       <c r="G30" s="6"/>
@@ -9062,7 +9059,7 @@
         <v>38430</v>
       </c>
       <c r="F31">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91753414191576732</v>
       </c>
       <c r="G31" s="6"/>
@@ -9093,7 +9090,7 @@
         <v>40660</v>
       </c>
       <c r="F32">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97093870143515537</v>
       </c>
       <c r="G32" s="6"/>
@@ -9124,7 +9121,7 @@
         <v>38810</v>
       </c>
       <c r="F33">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92685023762328944</v>
       </c>
       <c r="G33" s="6"/>
@@ -9155,7 +9152,7 @@
         <v>40910</v>
       </c>
       <c r="F34">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97718858234802342</v>
       </c>
       <c r="G34" s="6"/>
@@ -9186,7 +9183,7 @@
         <v>38570</v>
       </c>
       <c r="F35">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92142669437874769</v>
       </c>
       <c r="G35" s="6"/>
@@ -9217,7 +9214,7 @@
         <v>39910</v>
       </c>
       <c r="F36">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95362117990012185</v>
       </c>
       <c r="G36" s="6"/>
@@ -9248,7 +9245,7 @@
         <v>39620</v>
       </c>
       <c r="F37">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94680495148879229</v>
       </c>
       <c r="G37" s="6"/>
@@ -9279,7 +9276,7 @@
         <v>40230</v>
       </c>
       <c r="F38">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96156604044170368</v>
       </c>
       <c r="G38" s="6"/>
@@ -9310,7 +9307,7 @@
         <v>39030</v>
       </c>
       <c r="F39">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93299548203571347</v>
       </c>
       <c r="G39" s="6"/>
@@ -9341,7 +9338,7 @@
         <v>39840</v>
       </c>
       <c r="F40">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95247202830639766</v>
       </c>
       <c r="G40" s="6"/>
@@ -9372,7 +9369,7 @@
         <v>39640</v>
       </c>
       <c r="F41">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94787183165949307</v>
       </c>
       <c r="G41" s="6"/>
@@ -9403,7 +9400,7 @@
         <v>39620</v>
       </c>
       <c r="F42">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94755219668524138</v>
       </c>
       <c r="G42" s="6"/>
@@ -9434,7 +9431,7 @@
         <v>40110</v>
       </c>
       <c r="F43">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9594775619557937</v>
       </c>
       <c r="G43" s="6"/>
@@ -9465,7 +9462,7 @@
         <v>40390</v>
       </c>
       <c r="F44">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96633729693518677</v>
       </c>
       <c r="G44" s="6"/>
@@ -9496,7 +9493,7 @@
         <v>39870</v>
       </c>
       <c r="F45">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95407882457105941</v>
       </c>
       <c r="G45" s="6"/>
@@ -9527,7 +9524,7 @@
         <v>39800</v>
       </c>
       <c r="F46">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95265450715687683</v>
       </c>
       <c r="G46" s="6"/>
@@ -9558,7 +9555,7 @@
         <v>40130</v>
       </c>
       <c r="F47">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96085238836346221</v>
       </c>
       <c r="G47" s="6"/>
@@ -9589,7 +9586,7 @@
         <v>40230</v>
       </c>
       <c r="F48">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96363897671744758</v>
       </c>
       <c r="G48" s="6"/>
@@ -9620,7 +9617,7 @@
         <v>40650</v>
       </c>
       <c r="F49">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9740026356774889</v>
       </c>
       <c r="G49" s="6"/>
@@ -9651,7 +9648,7 @@
         <v>40290</v>
       </c>
       <c r="F50">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96558500695010308</v>
       </c>
       <c r="G50" s="6"/>
@@ -9682,7 +9679,7 @@
         <v>39790</v>
       </c>
       <c r="F51">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95371635387454756</v>
       </c>
       <c r="G51" s="6"/>
@@ -9713,7 +9710,7 @@
         <v>40700</v>
       </c>
       <c r="F52">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.975715004914535</v>
       </c>
       <c r="G52" s="6"/>
@@ -9744,7 +9741,7 @@
         <v>40430</v>
       </c>
       <c r="F53">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96940488179158879</v>
       </c>
       <c r="G53" s="6"/>
@@ -9775,7 +9772,7 @@
         <v>40770</v>
       </c>
       <c r="F54">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97779163468917885</v>
       </c>
       <c r="G54" s="6"/>
@@ -9806,7 +9803,7 @@
         <v>40190</v>
       </c>
       <c r="F55">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96397390386644921</v>
       </c>
       <c r="G55" s="6"/>
@@ -9837,7 +9834,7 @@
         <v>40450</v>
       </c>
       <c r="F56">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97037303586421975</v>
       </c>
       <c r="G56" s="6"/>
@@ -9868,7 +9865,7 @@
         <v>40420</v>
       </c>
       <c r="F57">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96976967370441458</v>
       </c>
       <c r="G57" s="6"/>
@@ -9899,7 +9896,7 @@
         <v>40630</v>
       </c>
       <c r="F58">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97494840908000191</v>
       </c>
       <c r="G58" s="6"/>
@@ -9930,7 +9927,7 @@
         <v>39920</v>
       </c>
       <c r="F59">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95809532952527243</v>
       </c>
       <c r="G59" s="6"/>
@@ -9961,7 +9958,7 @@
         <v>40490</v>
       </c>
       <c r="F60">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97203216900732203</v>
       </c>
       <c r="G60" s="6"/>
@@ -9992,7 +9989,7 @@
         <v>40460</v>
       </c>
       <c r="F61">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97154520350582307</v>
       </c>
       <c r="G61" s="6"/>
@@ -10023,7 +10020,7 @@
         <v>40130</v>
       </c>
       <c r="F62">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96378308276093949</v>
       </c>
       <c r="G62" s="6"/>
@@ -10054,7 +10051,7 @@
         <v>40250</v>
       </c>
       <c r="F63">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96675793822356726</v>
       </c>
       <c r="G63" s="6"/>
@@ -10085,7 +10082,7 @@
         <v>40660</v>
       </c>
       <c r="F64">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97679335030990244</v>
       </c>
       <c r="G64" s="6"/>
@@ -10116,7 +10113,7 @@
         <v>39840</v>
       </c>
       <c r="F65">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95727810082175979</v>
       </c>
       <c r="G65" s="6"/>
@@ -10147,7 +10144,7 @@
         <v>39980</v>
       </c>
       <c r="F66">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96080363365456245</v>
       </c>
       <c r="G66" s="6"/>
@@ -10178,7 +10175,7 @@
         <v>40630</v>
       </c>
       <c r="F67">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97654184492621254</v>
       </c>
       <c r="G67" s="6"/>
@@ -10209,7 +10206,7 @@
         <v>41170</v>
       </c>
       <c r="F68">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98968725209740616</v>
       </c>
       <c r="G68" s="6"/>
@@ -10240,7 +10237,7 @@
         <v>40070</v>
       </c>
       <c r="F69">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96336010001442518</v>
       </c>
       <c r="G69" s="6"/>
@@ -10271,7 +10268,7 @@
         <v>40230</v>
       </c>
       <c r="F70">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96732309024020779</v>
       </c>
       <c r="G70" s="6"/>
@@ -10302,7 +10299,7 @@
         <v>40540</v>
       </c>
       <c r="F71">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97496452706765113</v>
       </c>
       <c r="G71" s="6"/>
@@ -10333,7 +10330,7 @@
         <v>41000</v>
       </c>
       <c r="F72">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98624073895891462</v>
       </c>
       <c r="G72" s="6"/>
@@ -10364,7 +10361,7 @@
         <v>39920</v>
       </c>
       <c r="F73">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96042343317695178</v>
       </c>
       <c r="G73" s="6"/>
@@ -10395,7 +10392,7 @@
         <v>40760</v>
       </c>
       <c r="F74">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98086872819155335</v>
       </c>
       <c r="G74" s="6"/>
@@ -10426,7 +10423,7 @@
         <v>40590</v>
       </c>
       <c r="F75">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97694233176085488</v>
       </c>
       <c r="G75" s="6"/>
@@ -10457,7 +10454,7 @@
         <v>40290</v>
       </c>
       <c r="F76">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96990852190659604</v>
       </c>
       <c r="G76" s="6"/>
@@ -10488,7 +10485,7 @@
         <v>39780</v>
       </c>
       <c r="F77">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95786178666024557</v>
       </c>
       <c r="G77" s="6"/>
@@ -10519,7 +10516,7 @@
         <v>40780</v>
       </c>
       <c r="F78">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98236654461360573</v>
       </c>
       <c r="G78" s="6"/>
@@ -10550,7 +10547,7 @@
         <v>40490</v>
       </c>
       <c r="F79">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97556861989205856</v>
       </c>
       <c r="G79" s="6"/>
@@ -10581,7 +10578,7 @@
         <v>39690</v>
       </c>
       <c r="F80">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95668522669751965</v>
       </c>
       <c r="G80" s="6"/>
@@ -10612,7 +10609,7 @@
         <v>40370</v>
       </c>
       <c r="F81">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97354522873610339</v>
       </c>
       <c r="G81" s="6"/>
@@ -10643,7 +10640,7 @@
         <v>40180</v>
       </c>
       <c r="F82">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96926713947990539</v>
       </c>
       <c r="G82" s="6"/>
@@ -10674,7 +10671,7 @@
         <v>39870</v>
       </c>
       <c r="F83">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96197461757467551</v>
       </c>
       <c r="G83" s="6"/>
@@ -10705,7 +10702,7 @@
         <v>39340</v>
       </c>
       <c r="F84">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94955346367366644</v>
       </c>
       <c r="G84" s="6"/>
@@ -10736,7 +10733,7 @@
         <v>40520</v>
       </c>
       <c r="F85">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97824774872649134</v>
       </c>
       <c r="G85" s="6"/>
@@ -10767,7 +10764,7 @@
         <v>41330</v>
       </c>
       <c r="F86">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99818862456225088</v>
       </c>
       <c r="G86" s="6"/>
@@ -10798,7 +10795,7 @@
         <v>37460</v>
       </c>
       <c r="F87">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90494021017031046</v>
       </c>
       <c r="G87" s="6"/>
@@ -10829,7 +10826,7 @@
         <v>40170</v>
       </c>
       <c r="F88">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97057118005218901</v>
       </c>
       <c r="G88" s="6"/>
@@ -10860,7 +10857,7 @@
         <v>40370</v>
       </c>
       <c r="F89">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9756392285755715</v>
       </c>
       <c r="G89" s="6"/>
@@ -10891,7 +10888,7 @@
         <v>40890</v>
       </c>
       <c r="F90">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98856465923651571</v>
       </c>
       <c r="G90" s="6"/>
@@ -10922,7 +10919,7 @@
         <v>39900</v>
       </c>
       <c r="F91">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96479350033852407</v>
       </c>
       <c r="G91" s="6"/>
@@ -10953,7 +10950,7 @@
         <v>39660</v>
       </c>
       <c r="F92">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95912938331318021</v>
       </c>
       <c r="G92" s="6"/>
@@ -10984,7 +10981,7 @@
         <v>40090</v>
       </c>
       <c r="F93">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96973948380542319</v>
       </c>
       <c r="G93" s="6"/>
@@ -11015,7 +11012,7 @@
         <v>39300</v>
       </c>
       <c r="F94">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95083712377818641</v>
       </c>
       <c r="G94" s="6"/>
@@ -11046,7 +11043,7 @@
         <v>39630</v>
       </c>
       <c r="F95">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95891405342624858</v>
       </c>
       <c r="G95" s="6"/>
@@ -11077,7 +11074,7 @@
         <v>40350</v>
       </c>
       <c r="F96">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97659559019289877</v>
       </c>
       <c r="G96" s="6"/>
@@ -11108,7 +11105,7 @@
         <v>40960</v>
       </c>
       <c r="F97">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99167150881270583</v>
       </c>
       <c r="G97" s="6"/>
@@ -11139,7 +11136,7 @@
         <v>40070</v>
       </c>
       <c r="F98">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97047639807212571</v>
       </c>
       <c r="G98" s="6"/>
@@ -11170,7 +11167,7 @@
         <v>37840</v>
       </c>
       <c r="F99">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91675549956391122</v>
       </c>
       <c r="G99" s="6"/>
@@ -11201,7 +11198,7 @@
         <v>40630</v>
       </c>
       <c r="F100">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98446851299944271</v>
       </c>
       <c r="G100" s="6"/>
@@ -11232,7 +11229,7 @@
         <v>37370</v>
       </c>
       <c r="F101">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90569787450619232</v>
       </c>
       <c r="G101" s="6"/>
@@ -11263,7 +11260,7 @@
         <v>39990</v>
       </c>
       <c r="F102">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96936054685606243</v>
       </c>
       <c r="G102" s="6"/>
@@ -11294,7 +11291,7 @@
         <v>40960</v>
       </c>
       <c r="F103">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99311414993696057</v>
       </c>
       <c r="G103" s="6"/>
@@ -11325,7 +11322,7 @@
         <v>40660</v>
       </c>
       <c r="F104">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98598380134827102</v>
       </c>
       <c r="G104" s="6"/>
@@ -11356,7 +11353,7 @@
         <v>39770</v>
       </c>
       <c r="F105">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96456549683490578</v>
       </c>
       <c r="G105" s="6"/>
@@ -11387,7 +11384,7 @@
         <v>40100</v>
       </c>
       <c r="F106">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97275792640031056</v>
       </c>
       <c r="G106" s="6"/>
@@ -11418,7 +11415,7 @@
         <v>40130</v>
       </c>
       <c r="F107">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97360376534523752</v>
       </c>
       <c r="G107" s="6"/>
@@ -11449,7 +11446,7 @@
         <v>40430</v>
       </c>
       <c r="F108">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98104874912038043</v>
       </c>
       <c r="G108" s="6"/>
@@ -11480,7 +11477,7 @@
         <v>39580</v>
       </c>
       <c r="F109">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96060966434482931</v>
       </c>
       <c r="G109" s="6"/>
@@ -11511,7 +11508,7 @@
         <v>39680</v>
       </c>
       <c r="F110">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96320031070977763</v>
       </c>
       <c r="G110" s="6"/>
@@ -11542,7 +11539,7 @@
         <v>40380</v>
       </c>
       <c r="F111">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98035883366918353</v>
       </c>
       <c r="G111" s="6"/>
@@ -11573,7 +11570,7 @@
         <v>38500</v>
       </c>
       <c r="F112">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93494256781369145</v>
       </c>
       <c r="G112" s="6"/>
@@ -11604,7 +11601,7 @@
         <v>40750</v>
       </c>
       <c r="F113">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98984648270501363</v>
       </c>
       <c r="G113" s="6"/>
@@ -11635,7 +11632,7 @@
         <v>40310</v>
       </c>
       <c r="F114">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97939647213178482</v>
       </c>
       <c r="G114" s="6"/>
@@ -11666,7 +11663,7 @@
         <v>39490</v>
       </c>
       <c r="F115">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95972974943495271</v>
       </c>
       <c r="G115" s="6"/>
@@ -11697,7 +11694,7 @@
         <v>39620</v>
       </c>
       <c r="F116">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96312322240318937</v>
       </c>
       <c r="G116" s="6"/>
@@ -11728,7 +11725,7 @@
         <v>40540</v>
       </c>
       <c r="F117">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98567920445427804</v>
       </c>
       <c r="G117" s="6"/>
@@ -11759,7 +11756,7 @@
         <v>40020</v>
       </c>
       <c r="F118">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97317802689492494</v>
       </c>
       <c r="G118" s="6"/>
@@ -11790,7 +11787,7 @@
         <v>38860</v>
       </c>
       <c r="F119">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94529178525383739</v>
       </c>
       <c r="G119" s="6"/>
@@ -11821,7 +11818,7 @@
         <v>39550</v>
       </c>
       <c r="F120">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96231051850409988</v>
       </c>
       <c r="G120" s="6"/>
@@ -11852,7 +11849,7 @@
         <v>40970</v>
       </c>
       <c r="F121">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99703105227294853</v>
       </c>
       <c r="G121" s="6"/>
@@ -11883,7 +11880,7 @@
         <v>40970</v>
       </c>
       <c r="F122">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99717665384802612</v>
       </c>
       <c r="G122" s="6"/>
@@ -11914,7 +11911,7 @@
         <v>40580</v>
       </c>
       <c r="F123">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98780458119325232</v>
       </c>
       <c r="G123" s="6"/>
@@ -11945,7 +11942,7 @@
         <v>39880</v>
       </c>
       <c r="F124">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97104872288100519</v>
       </c>
       <c r="G124" s="6"/>
@@ -11976,7 +11973,7 @@
         <v>39850</v>
       </c>
       <c r="F125">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97043639197350473</v>
       </c>
       <c r="G125" s="6"/>
@@ -12007,7 +12004,7 @@
         <v>40390</v>
       </c>
       <c r="F126">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98375429281243154</v>
       </c>
       <c r="G126" s="6"/>
@@ -12038,7 +12035,7 @@
         <v>39220</v>
       </c>
       <c r="F127">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95544349436039855</v>
       </c>
       <c r="G127" s="6"/>
@@ -12069,7 +12066,7 @@
         <v>40800</v>
       </c>
       <c r="F128">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99415204678362568</v>
       </c>
       <c r="G128" s="6"/>
@@ -12100,7 +12097,7 @@
         <v>40680</v>
       </c>
       <c r="F129">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99137300774967096</v>
       </c>
       <c r="G129" s="6"/>
@@ -12131,7 +12128,7 @@
         <v>39110</v>
       </c>
       <c r="F130">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95327467277646427</v>
       </c>
       <c r="G130" s="6"/>
@@ -12162,7 +12159,7 @@
         <v>38870</v>
       </c>
       <c r="F131">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94751724642273849</v>
       </c>
       <c r="G131" s="6"/>
@@ -12193,7 +12190,7 @@
         <v>40380</v>
       </c>
       <c r="F132">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9845658693584961</v>
       </c>
       <c r="G132" s="6"/>
@@ -12224,7 +12221,7 @@
         <v>40200</v>
       </c>
       <c r="F133">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98034433985270453</v>
       </c>
       <c r="G133" s="6"/>
@@ -12255,7 +12252,7 @@
         <v>37640</v>
       </c>
       <c r="F134">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91820554728856141</v>
       </c>
       <c r="G134" s="6"/>
@@ -12286,7 +12283,7 @@
         <v>38180</v>
       </c>
       <c r="F135">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93156032694888369</v>
       </c>
       <c r="G135" s="6"/>
@@ -12317,7 +12314,7 @@
         <v>40900</v>
       </c>
       <c r="F136">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99804782820888238</v>
       </c>
       <c r="G136" s="6"/>
@@ -12348,7 +12345,7 @@
         <v>37740</v>
       </c>
       <c r="F137">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92111686029483553</v>
       </c>
       <c r="G137" s="6"/>
@@ -12379,7 +12376,7 @@
         <v>38360</v>
       </c>
       <c r="F138">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9364548494983278</v>
       </c>
       <c r="G138" s="6"/>
@@ -12410,7 +12407,7 @@
         <v>39580</v>
       </c>
       <c r="F139">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96649736276616527</v>
       </c>
       <c r="G139" s="6"/>
@@ -12441,7 +12438,7 @@
         <v>40050</v>
       </c>
       <c r="F140">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97828476513837659</v>
       </c>
       <c r="G140" s="6"/>
@@ -12472,7 +12469,7 @@
         <v>38350</v>
       </c>
       <c r="F141">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93705712749841175</v>
       </c>
       <c r="G141" s="6"/>
@@ -12503,7 +12500,7 @@
         <v>40400</v>
       </c>
       <c r="F142">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9874853343762221</v>
       </c>
       <c r="G142" s="6"/>
@@ -12534,7 +12531,7 @@
         <v>35340</v>
       </c>
       <c r="F143">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8641854550789847</v>
       </c>
       <c r="G143" s="6"/>
@@ -12565,7 +12562,7 @@
         <v>38430</v>
       </c>
       <c r="F144">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93995352818882227</v>
       </c>
       <c r="G144" s="6"/>
@@ -12596,7 +12593,7 @@
         <v>38220</v>
       </c>
       <c r="F145">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93506874785927485</v>
       </c>
       <c r="G145" s="6"/>
@@ -12627,7 +12624,7 @@
         <v>40470</v>
       </c>
       <c r="F146">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99033402667319226</v>
       </c>
       <c r="G146" s="6"/>
@@ -12658,7 +12655,7 @@
         <v>38280</v>
       </c>
       <c r="F147">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93694928529469357</v>
       </c>
       <c r="G147" s="6"/>
@@ -12689,7 +12686,7 @@
         <v>40540</v>
       </c>
       <c r="F148">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99250844635949664</v>
       </c>
       <c r="G148" s="6"/>
@@ -12720,7 +12717,7 @@
         <v>37510</v>
       </c>
       <c r="F149">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91857475205093675</v>
       </c>
       <c r="G149" s="6"/>
@@ -12751,7 +12748,7 @@
         <v>34520</v>
       </c>
       <c r="F150">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.84558103076621594</v>
       </c>
       <c r="G150" s="6"/>
@@ -12782,7 +12779,7 @@
         <v>38300</v>
       </c>
       <c r="F151">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93831152922730165</v>
       </c>
       <c r="G151" s="6"/>
@@ -12813,7 +12810,7 @@
         <v>37860</v>
       </c>
       <c r="F152">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92778199818658569</v>
       </c>
       <c r="G152" s="6"/>
@@ -12844,7 +12841,7 @@
         <v>32260</v>
       </c>
       <c r="F153">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79064751727856475</v>
       </c>
       <c r="G153" s="6"/>
@@ -12875,7 +12872,7 @@
         <v>37650</v>
       </c>
       <c r="F154">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92288459652907151</v>
       </c>
       <c r="G154" s="6"/>
@@ -12906,7 +12903,7 @@
         <v>36900</v>
       </c>
       <c r="F155">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90474439132033835</v>
       </c>
       <c r="G155" s="6"/>
@@ -12937,7 +12934,7 @@
         <v>39990</v>
       </c>
       <c r="F156">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98067585462749518</v>
       </c>
       <c r="G156" s="6"/>
@@ -12968,7 +12965,7 @@
         <v>37500</v>
       </c>
       <c r="F157">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91981652726336183</v>
       </c>
       <c r="G157" s="6"/>
@@ -12999,7 +12996,7 @@
         <v>37900</v>
       </c>
       <c r="F158">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92983316977428854</v>
       </c>
       <c r="G158" s="6"/>
@@ -13030,7 +13027,7 @@
         <v>38370</v>
       </c>
       <c r="F159">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94159509202453984</v>
       </c>
       <c r="G159" s="6"/>
@@ -13061,7 +13058,7 @@
         <v>40380</v>
       </c>
       <c r="F160">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99121213608915504</v>
       </c>
       <c r="G160" s="6"/>
@@ -13092,7 +13089,7 @@
         <v>35010</v>
       </c>
       <c r="F161">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85964739969552617</v>
       </c>
       <c r="G161" s="6"/>
@@ -13123,7 +13120,7 @@
         <v>38850</v>
       </c>
       <c r="F162">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95405319122811327</v>
       </c>
       <c r="G162" s="6"/>
@@ -13154,7 +13151,7 @@
         <v>37590</v>
       </c>
       <c r="F163">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92331499312242094</v>
       </c>
       <c r="G163" s="6"/>
@@ -13185,7 +13182,7 @@
         <v>38730</v>
       </c>
       <c r="F164">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95155029236892541</v>
       </c>
       <c r="G164" s="6"/>
@@ -13216,7 +13213,7 @@
         <v>40470</v>
       </c>
       <c r="F165">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99459326615876131</v>
       </c>
       <c r="G165" s="6"/>
@@ -13247,7 +13244,7 @@
         <v>38190</v>
       </c>
       <c r="F166">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93872133323501217</v>
       </c>
       <c r="G166" s="6"/>
@@ -13278,7 +13275,7 @@
         <v>40230</v>
       </c>
       <c r="F167">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98908393568372921</v>
       </c>
       <c r="G167" s="6"/>
@@ -13309,7 +13306,7 @@
         <v>33940</v>
       </c>
       <c r="F168">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.83456280121963211</v>
       </c>
       <c r="G168" s="6"/>
@@ -13340,7 +13337,7 @@
         <v>37940</v>
       </c>
       <c r="F169">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93310378750614853</v>
       </c>
       <c r="G169" s="6"/>
@@ -13371,7 +13368,7 @@
         <v>40000</v>
       </c>
       <c r="F170">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98391302208884734</v>
       </c>
       <c r="G170" s="6"/>
@@ -13402,7 +13399,7 @@
         <v>36960</v>
       </c>
       <c r="F171">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90935931502804845</v>
       </c>
       <c r="G171" s="6"/>
@@ -13433,7 +13430,7 @@
         <v>40050</v>
       </c>
       <c r="F172">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9857490954736764</v>
       </c>
       <c r="G172" s="6"/>
@@ -13464,7 +13461,7 @@
         <v>37110</v>
       </c>
       <c r="F173">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91354438481610944</v>
       </c>
       <c r="G173" s="6"/>
@@ -13495,7 +13492,7 @@
         <v>39000</v>
       </c>
       <c r="F174">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96028365301750673</v>
       </c>
       <c r="G174" s="6"/>
@@ -13526,7 +13523,7 @@
         <v>36660</v>
       </c>
       <c r="F175">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90293342528509146</v>
       </c>
       <c r="G175" s="6"/>
@@ -13557,7 +13554,7 @@
         <v>39870</v>
       </c>
       <c r="F176">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98240685984624487</v>
       </c>
       <c r="G176" s="6"/>
@@ -13588,7 +13585,7 @@
         <v>36320</v>
       </c>
       <c r="F177">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89530899499593264</v>
       </c>
       <c r="G177" s="6"/>
@@ -13619,7 +13616,7 @@
         <v>38930</v>
       </c>
       <c r="F178">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95985995364662957</v>
       </c>
       <c r="G178" s="6"/>
@@ -13650,7 +13647,7 @@
         <v>39710</v>
       </c>
       <c r="F179">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97952639368524919</v>
       </c>
       <c r="G179" s="6"/>
@@ -13681,7 +13678,7 @@
         <v>36340</v>
       </c>
       <c r="F180">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89657554524819894</v>
       </c>
       <c r="G180" s="6"/>
@@ -13712,7 +13709,7 @@
         <v>38820</v>
       </c>
       <c r="F181">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95806905402403808</v>
       </c>
       <c r="G181" s="6"/>
@@ -13743,7 +13740,7 @@
         <v>39210</v>
       </c>
       <c r="F182">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96807643878231242</v>
       </c>
       <c r="G182" s="6"/>
@@ -13774,7 +13771,7 @@
         <v>39990</v>
       </c>
       <c r="F183">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98770005927682281</v>
       </c>
       <c r="G183" s="6"/>
@@ -13805,7 +13802,7 @@
         <v>39810</v>
       </c>
       <c r="F184">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98359440628551664</v>
       </c>
       <c r="G184" s="6"/>
@@ -13836,7 +13833,7 @@
         <v>38880</v>
       </c>
       <c r="F185">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96106785317018906</v>
       </c>
       <c r="G185" s="6"/>
@@ -13867,7 +13864,7 @@
         <v>35190</v>
       </c>
       <c r="F186">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87011349306431274</v>
       </c>
       <c r="G186" s="6"/>
@@ -13898,7 +13895,7 @@
         <v>38190</v>
       </c>
       <c r="F187">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9446656937195439</v>
       </c>
       <c r="G187" s="6"/>
@@ -13929,7 +13926,7 @@
         <v>40000</v>
       </c>
       <c r="F188">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98965807313573162</v>
       </c>
       <c r="G188" s="6"/>
@@ -13960,7 +13957,7 @@
         <v>34120</v>
       </c>
       <c r="F189">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8445962671419377</v>
       </c>
       <c r="G189" s="6"/>
@@ -13991,7 +13988,7 @@
         <v>37380</v>
       </c>
       <c r="F190">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92554534875083572</v>
       </c>
       <c r="G190" s="6"/>
@@ -14022,7 +14019,7 @@
         <v>35400</v>
       </c>
       <c r="F191">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87678018575851391</v>
       </c>
       <c r="G191" s="6"/>
@@ -14053,7 +14050,7 @@
         <v>38900</v>
       </c>
       <c r="F192">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96389721733528255</v>
       </c>
       <c r="G192" s="6"/>
@@ -14084,7 +14081,7 @@
         <v>39790</v>
       </c>
       <c r="F193">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98621920388638273</v>
       </c>
       <c r="G193" s="6"/>
@@ -14115,7 +14112,7 @@
         <v>36090</v>
       </c>
       <c r="F194">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89491172386431261</v>
       </c>
       <c r="G194" s="6"/>
@@ -14146,7 +14143,7 @@
         <v>36540</v>
       </c>
       <c r="F195">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90636239613047254</v>
       </c>
       <c r="G195" s="6"/>
@@ -14177,7 +14174,7 @@
         <v>36690</v>
       </c>
       <c r="F196">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91021856161155079</v>
       </c>
       <c r="G196" s="6"/>
@@ -14208,7 +14205,7 @@
         <v>37290</v>
       </c>
       <c r="F197">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92537906047596596</v>
       </c>
       <c r="G197" s="6"/>
@@ -14239,7 +14236,7 @@
         <v>38610</v>
       </c>
       <c r="F198">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95854021847070503</v>
       </c>
       <c r="G198" s="6"/>
@@ -14270,7 +14267,7 @@
         <v>38070</v>
       </c>
       <c r="F199">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94553311973772447</v>
       </c>
       <c r="G199" s="6"/>
@@ -14301,7 +14298,7 @@
         <v>36600</v>
       </c>
       <c r="F200">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9092038256117253</v>
       </c>
       <c r="G200" s="6"/>
@@ -14332,7 +14329,7 @@
         <v>40090</v>
       </c>
       <c r="F201">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99619809656337743</v>
       </c>
       <c r="G201" s="6"/>
@@ -14363,7 +14360,7 @@
         <v>36410</v>
       </c>
       <c r="F202">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90502348934900945</v>
       </c>
       <c r="G202" s="6"/>
@@ -14394,7 +14391,7 @@
         <v>36660</v>
       </c>
       <c r="F203">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91155481512793102</v>
       </c>
       <c r="G203" s="6"/>
@@ -14425,7 +14422,7 @@
         <v>35750</v>
       </c>
       <c r="F204">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88908231783138525</v>
       </c>
       <c r="G204" s="6"/>
@@ -14456,7 +14453,7 @@
         <v>39060</v>
       </c>
       <c r="F205">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97169013383750436</v>
       </c>
       <c r="G205" s="6"/>
@@ -14487,7 +14484,7 @@
         <v>38070</v>
       </c>
       <c r="F206">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94722699111741437</v>
       </c>
       <c r="G206" s="6"/>
@@ -14518,7 +14515,7 @@
         <v>36300</v>
       </c>
       <c r="F207">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90341206042656974</v>
       </c>
       <c r="G207" s="6"/>
@@ -14549,7 +14546,7 @@
         <v>39540</v>
       </c>
       <c r="F208">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98416965352449226</v>
       </c>
       <c r="G208" s="6"/>
@@ -14580,7 +14577,7 @@
         <v>36450</v>
       </c>
       <c r="F209">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90757432398784921</v>
       </c>
       <c r="G209" s="6"/>
@@ -14611,7 +14608,7 @@
         <v>37080</v>
       </c>
       <c r="F210">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92339874489490981</v>
       </c>
       <c r="G210" s="6"/>
@@ -14642,7 +14639,7 @@
         <v>35400</v>
       </c>
       <c r="F211">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88186936375865677</v>
       </c>
       <c r="G211" s="6"/>
@@ -14673,7 +14670,7 @@
         <v>37560</v>
       </c>
       <c r="F212">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93577158802132643</v>
       </c>
       <c r="G212" s="6"/>
@@ -14704,7 +14701,7 @@
         <v>39150</v>
       </c>
       <c r="F213">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97565230393500635</v>
       </c>
       <c r="G213" s="6"/>
@@ -14735,7 +14732,7 @@
         <v>37890</v>
       </c>
       <c r="F214">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94444029013684294</v>
       </c>
       <c r="G214" s="6"/>
@@ -14766,7 +14763,7 @@
         <v>36780</v>
       </c>
       <c r="F215">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91688687241362121</v>
       </c>
       <c r="G215" s="6"/>
@@ -14797,7 +14794,7 @@
         <v>35220</v>
       </c>
       <c r="F216">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87826043588848435</v>
       </c>
       <c r="G216" s="6"/>
@@ -14828,7 +14825,7 @@
         <v>36540</v>
       </c>
       <c r="F217">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91149471163440432</v>
       </c>
       <c r="G217" s="6"/>
@@ -14859,7 +14856,7 @@
         <v>38310</v>
       </c>
       <c r="F218">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95593372592075054</v>
       </c>
       <c r="G218" s="6"/>
@@ -14890,7 +14887,7 @@
         <v>39820</v>
       </c>
       <c r="F219">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99378571963363194</v>
       </c>
       <c r="G219" s="6"/>
@@ -14921,7 +14918,7 @@
         <v>35350</v>
       </c>
       <c r="F220">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88244838862677555</v>
       </c>
       <c r="G220" s="6"/>
@@ -14952,7 +14949,7 @@
         <v>35700</v>
       </c>
       <c r="F221">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89129674938832582</v>
       </c>
       <c r="G221" s="6"/>
@@ -14983,7 +14980,7 @@
         <v>39200</v>
       </c>
       <c r="F222">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97892318449705329</v>
       </c>
       <c r="G222" s="6"/>
@@ -15014,7 +15011,7 @@
         <v>36010</v>
       </c>
       <c r="F223">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89946296990133634</v>
       </c>
       <c r="G223" s="6"/>
@@ -15045,7 +15042,7 @@
         <v>38160</v>
       </c>
       <c r="F224">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95335648437304821</v>
       </c>
       <c r="G224" s="6"/>
@@ -15076,7 +15073,7 @@
         <v>38100</v>
       </c>
       <c r="F225">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95214294639510189</v>
       </c>
       <c r="G225" s="6"/>
@@ -15107,7 +15104,7 @@
         <v>37560</v>
       </c>
       <c r="F226">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93876530867283181</v>
       </c>
       <c r="G226" s="6"/>
@@ -15138,7 +15135,7 @@
         <v>35100</v>
       </c>
       <c r="F227">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8774561271936403</v>
       </c>
       <c r="G227" s="6"/>
@@ -15169,7 +15166,7 @@
         <v>39750</v>
       </c>
       <c r="F228">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99382453684026306</v>
       </c>
       <c r="G228" s="6"/>
@@ -15200,7 +15197,7 @@
         <v>35670</v>
       </c>
       <c r="F229">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89192838567713539</v>
       </c>
       <c r="G229" s="6"/>
@@ -15231,7 +15228,7 @@
         <v>38340</v>
       </c>
       <c r="F230">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95878763629088726</v>
       </c>
       <c r="G230" s="6"/>
@@ -15262,7 +15259,7 @@
         <v>35520</v>
       </c>
       <c r="F231">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8884220004502138</v>
       </c>
       <c r="G231" s="6"/>
@@ -15293,7 +15290,7 @@
         <v>35910</v>
       </c>
       <c r="F232">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8983339170460799</v>
       </c>
       <c r="G232" s="6"/>
@@ -15324,7 +15321,7 @@
         <v>35730</v>
       </c>
       <c r="F233">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89400990842215888</v>
       </c>
       <c r="G233" s="6"/>
@@ -15355,7 +15352,7 @@
         <v>38670</v>
       </c>
       <c r="F234">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96781459605566122</v>
       </c>
       <c r="G234" s="6"/>
@@ -15386,7 +15383,7 @@
         <v>35160</v>
       </c>
       <c r="F235">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88014418744367673</v>
       </c>
       <c r="G235" s="6"/>
@@ -15417,7 +15414,7 @@
         <v>37260</v>
       </c>
       <c r="F236">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93289934902353533</v>
       </c>
       <c r="G236" s="6"/>
@@ -15448,7 +15445,7 @@
         <v>39790</v>
       </c>
       <c r="F237">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99636909978715416</v>
       </c>
       <c r="G237" s="6"/>
@@ -15479,7 +15476,7 @@
         <v>35810</v>
       </c>
       <c r="F238">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89686435584051294</v>
       </c>
       <c r="G238" s="6"/>
@@ -15510,7 +15507,7 @@
         <v>36600</v>
       </c>
       <c r="F239">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91683366733466931</v>
       </c>
       <c r="G239" s="6"/>
@@ -15541,7 +15538,7 @@
         <v>35100</v>
       </c>
       <c r="F240">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87934662791862916</v>
       </c>
       <c r="G240" s="6"/>
@@ -15572,7 +15569,7 @@
         <v>37200</v>
       </c>
       <c r="F241">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93230746096589057</v>
       </c>
       <c r="G241" s="6"/>
@@ -15603,7 +15600,7 @@
         <v>38790</v>
       </c>
       <c r="F242">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97230229352049125</v>
       </c>
       <c r="G242" s="6"/>
@@ -15634,7 +15631,7 @@
         <v>37260</v>
       </c>
       <c r="F243">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93427948145733553</v>
       </c>
       <c r="G243" s="6"/>
@@ -15665,7 +15662,7 @@
         <v>37830</v>
       </c>
       <c r="F244">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94871473354231972</v>
       </c>
       <c r="G244" s="6"/>
@@ -15696,7 +15693,7 @@
         <v>38400</v>
       </c>
       <c r="F245">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96315433043216536</v>
       </c>
       <c r="G245" s="6"/>
@@ -15727,7 +15724,7 @@
         <v>35830</v>
       </c>
       <c r="F246">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89885103607445682</v>
       </c>
       <c r="G246" s="6"/>
@@ -15758,7 +15755,7 @@
         <v>39380</v>
       </c>
       <c r="F247">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98800742636359074</v>
       </c>
       <c r="G247" s="6"/>
@@ -15789,7 +15786,7 @@
         <v>37200</v>
       </c>
       <c r="F248">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93357090872587645</v>
       </c>
       <c r="G248" s="6"/>
@@ -15820,7 +15817,7 @@
         <v>36180</v>
       </c>
       <c r="F249">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90820091874388131</v>
       </c>
       <c r="G249" s="6"/>
@@ -15851,7 +15848,7 @@
         <v>35510</v>
       </c>
       <c r="F250">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89149427595902797</v>
       </c>
       <c r="G250" s="6"/>
@@ -15882,7 +15879,7 @@
         <v>36340</v>
       </c>
       <c r="F251">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91258381256121146</v>
       </c>
       <c r="G251" s="6"/>
@@ -15913,7 +15910,7 @@
         <v>39440</v>
       </c>
       <c r="F252">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99065608359288659</v>
       </c>
       <c r="G252" s="6"/>
@@ -15944,7 +15941,7 @@
         <v>36760</v>
       </c>
       <c r="F253">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92354847624550918</v>
       </c>
       <c r="G253" s="6"/>
@@ -15975,7 +15972,7 @@
         <v>38310</v>
       </c>
       <c r="F254">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96261118649178345</v>
       </c>
       <c r="G254" s="6"/>
@@ -16006,7 +16003,7 @@
         <v>39450</v>
       </c>
       <c r="F255">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99135548072573754</v>
       </c>
       <c r="G255" s="6"/>
@@ -16037,7 +16034,7 @@
         <v>31620</v>
       </c>
       <c r="F256">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79471197345933442</v>
       </c>
       <c r="G256" s="6"/>
@@ -16068,7 +16065,7 @@
         <v>39570</v>
       </c>
       <c r="F257">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.99467095671409178</v>
       </c>
       <c r="G257" s="6"/>
@@ -16099,7 +16096,7 @@
         <v>38040</v>
       </c>
       <c r="F258">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95645177511817359</v>
       </c>
       <c r="G258" s="6"/>
@@ -16130,7 +16127,7 @@
         <v>37350</v>
       </c>
       <c r="F259">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93933906745133544</v>
       </c>
       <c r="G259" s="6"/>
@@ -16161,7 +16158,7 @@
         <v>37650</v>
       </c>
       <c r="F260">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94705068544837123</v>
       </c>
       <c r="G260" s="6"/>
@@ -16192,7 +16189,7 @@
         <v>37790</v>
       </c>
       <c r="F261">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95069182389937112</v>
       </c>
       <c r="G261" s="6"/>
@@ -16223,7 +16220,7 @@
         <v>36310</v>
       </c>
       <c r="F262">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91366598726755743</v>
       </c>
       <c r="G262" s="6"/>
@@ -16254,7 +16251,7 @@
         <v>35940</v>
       </c>
       <c r="F263">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90449226123065307</v>
       </c>
       <c r="G263" s="6"/>
@@ -16285,7 +16282,7 @@
         <v>34980</v>
       </c>
       <c r="F264">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88055380742605416</v>
       </c>
       <c r="G264" s="6"/>
@@ -16316,7 +16313,7 @@
         <v>36720</v>
       </c>
       <c r="F265">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92444802497419498</v>
       </c>
       <c r="G265" s="6"/>
@@ -16347,7 +16344,7 @@
         <v>38970</v>
       </c>
       <c r="F266">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98138960940844644</v>
       </c>
       <c r="G266" s="6"/>
@@ -16378,7 +16375,7 @@
         <v>36870</v>
       </c>
       <c r="F267">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92869197249439561</v>
       </c>
       <c r="G267" s="6"/>
@@ -16409,7 +16406,7 @@
         <v>38370</v>
       </c>
       <c r="F268">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96662048116891297</v>
       </c>
       <c r="G268" s="6"/>
@@ -16440,7 +16437,7 @@
         <v>34470</v>
       </c>
       <c r="F269">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86848072562358281</v>
       </c>
       <c r="G269" s="6"/>
@@ -16471,7 +16468,7 @@
         <v>38100</v>
       </c>
       <c r="F270">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.96020565034401073</v>
       </c>
       <c r="G270" s="6"/>
@@ -16502,7 +16499,7 @@
         <v>38900</v>
       </c>
       <c r="F271">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98058986639778167</v>
       </c>
       <c r="G271" s="6"/>
@@ -16533,7 +16530,7 @@
         <v>36220</v>
       </c>
       <c r="F272">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91321668095406183</v>
       </c>
       <c r="G272" s="6"/>
@@ -16564,7 +16561,7 @@
         <v>36450</v>
       </c>
       <c r="F273">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91922427054699518</v>
       </c>
       <c r="G273" s="6"/>
@@ -16595,7 +16592,7 @@
         <v>33870</v>
       </c>
       <c r="F274">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85426755447941893</v>
       </c>
       <c r="G274" s="6"/>
@@ -16626,7 +16623,7 @@
         <v>35730</v>
       </c>
       <c r="F275">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90131678522778869</v>
       </c>
       <c r="G275" s="6"/>
@@ -16657,7 +16654,7 @@
         <v>34980</v>
       </c>
       <c r="F276">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88257556643286073</v>
       </c>
       <c r="G276" s="6"/>
@@ -16688,7 +16685,7 @@
         <v>37560</v>
       </c>
       <c r="F277">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9478385948974184</v>
       </c>
       <c r="G277" s="6"/>
@@ -16719,7 +16716,7 @@
         <v>37470</v>
       </c>
       <c r="F278">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94566287257401005</v>
       </c>
       <c r="G278" s="6"/>
@@ -16750,7 +16747,7 @@
         <v>35570</v>
       </c>
       <c r="F279">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89789221254575291</v>
       </c>
       <c r="G279" s="6"/>
@@ -16781,7 +16778,7 @@
         <v>35220</v>
       </c>
       <c r="F280">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88919185033704462</v>
       </c>
       <c r="G280" s="6"/>
@@ -16812,7 +16809,7 @@
         <v>36210</v>
       </c>
       <c r="F281">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91439393939393943</v>
       </c>
       <c r="G281" s="6"/>
@@ -16843,7 +16840,7 @@
         <v>36990</v>
       </c>
       <c r="F282">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93423245946355504</v>
       </c>
       <c r="G282" s="6"/>
@@ -16874,7 +16871,7 @@
         <v>37440</v>
       </c>
       <c r="F283">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94576502387147299</v>
       </c>
       <c r="G283" s="6"/>
@@ -16905,7 +16902,7 @@
         <v>36240</v>
       </c>
       <c r="F284">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91563708026984003</v>
       </c>
       <c r="G284" s="6"/>
@@ -16936,7 +16933,7 @@
         <v>37620</v>
       </c>
       <c r="F285">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95081635747864324</v>
       </c>
       <c r="G285" s="6"/>
@@ -16967,7 +16964,7 @@
         <v>34170</v>
       </c>
       <c r="F286">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86375126390293222</v>
       </c>
       <c r="G286" s="6"/>
@@ -16998,7 +16995,7 @@
         <v>39030</v>
       </c>
       <c r="F287">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98692694768250433</v>
       </c>
       <c r="G287" s="6"/>
@@ -17029,7 +17026,7 @@
         <v>34170</v>
       </c>
       <c r="F288">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86431932007891943</v>
       </c>
       <c r="G288" s="6"/>
@@ -17060,7 +17057,7 @@
         <v>38690</v>
       </c>
       <c r="F289">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97879983808945559</v>
       </c>
       <c r="G289" s="6"/>
@@ -17091,7 +17088,7 @@
         <v>33100</v>
       </c>
       <c r="F290">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.83750822326805319</v>
       </c>
       <c r="G290" s="6"/>
@@ -17122,7 +17119,7 @@
         <v>35250</v>
       </c>
       <c r="F291">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89199858292423706</v>
       </c>
       <c r="G291" s="6"/>
@@ -17153,7 +17150,7 @@
         <v>38940</v>
       </c>
       <c r="F292">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.98552338530066819</v>
       </c>
       <c r="G292" s="6"/>
@@ -17184,7 +17181,7 @@
         <v>33660</v>
       </c>
       <c r="F293">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85210875398713992</v>
       </c>
       <c r="G293" s="6"/>
@@ -17215,7 +17212,7 @@
         <v>36840</v>
       </c>
       <c r="F294">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93282353834856813</v>
       </c>
       <c r="G294" s="6"/>
@@ -17246,7 +17243,7 @@
         <v>36720</v>
       </c>
       <c r="F295">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92999696079424576</v>
       </c>
       <c r="G295" s="6"/>
@@ -17277,7 +17274,7 @@
         <v>36000</v>
       </c>
       <c r="F296">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91190029890065349</v>
       </c>
       <c r="G296" s="6"/>
@@ -17308,7 +17305,7 @@
         <v>38660</v>
       </c>
       <c r="F297">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.97947808462123132</v>
       </c>
       <c r="G297" s="6"/>
@@ -17339,7 +17336,7 @@
         <v>36420</v>
       </c>
       <c r="F298">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.9228664098925603</v>
       </c>
       <c r="G298" s="6"/>
@@ -17370,7 +17367,7 @@
         <v>35820</v>
       </c>
       <c r="F299">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90789273584427432</v>
       </c>
       <c r="G299" s="6"/>
@@ -17401,7 +17398,7 @@
         <v>35820</v>
       </c>
       <c r="F300">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90800780754898724</v>
       </c>
       <c r="G300" s="6"/>
@@ -17432,7 +17429,7 @@
         <v>36000</v>
       </c>
       <c r="F301">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91277890466531442</v>
       </c>
       <c r="G301" s="6"/>
@@ -17463,7 +17460,7 @@
         <v>35670</v>
       </c>
       <c r="F302">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90454937363696297</v>
       </c>
       <c r="G302" s="6"/>
@@ -17494,7 +17491,7 @@
         <v>35400</v>
       </c>
       <c r="F303">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89795297161555432</v>
       </c>
       <c r="G303" s="6"/>
@@ -17525,7 +17522,7 @@
         <v>36390</v>
       </c>
       <c r="F304">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92351030352248498</v>
       </c>
       <c r="G304" s="6"/>
@@ -17556,7 +17553,7 @@
         <v>36630</v>
       </c>
       <c r="F305">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92976622585476054</v>
       </c>
       <c r="G305" s="6"/>
@@ -17587,7 +17584,7 @@
         <v>34710</v>
       </c>
       <c r="F306">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88129998730481152</v>
       </c>
       <c r="G306" s="6"/>
@@ -17618,7 +17615,7 @@
         <v>37020</v>
       </c>
       <c r="F307">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.94014272290931256</v>
       </c>
       <c r="G307" s="6"/>
@@ -17649,7 +17646,7 @@
         <v>33090</v>
       </c>
       <c r="F308">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.84044498628466935</v>
       </c>
       <c r="G308" s="6"/>
@@ -17680,7 +17677,7 @@
         <v>35460</v>
       </c>
       <c r="F309">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90086885828972108</v>
       </c>
       <c r="G309" s="6"/>
@@ -17711,7 +17708,7 @@
         <v>37530</v>
       </c>
       <c r="F310">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.95355455053610449</v>
       </c>
       <c r="G310" s="6"/>
@@ -17742,7 +17739,7 @@
         <v>34650</v>
       </c>
       <c r="F311">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88064860468662631</v>
       </c>
       <c r="G311" s="6"/>
@@ -17773,7 +17770,7 @@
         <v>35250</v>
       </c>
       <c r="F312">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89612568639414281</v>
       </c>
       <c r="G312" s="6"/>
@@ -17804,7 +17801,7 @@
         <v>34830</v>
       </c>
       <c r="F313">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88587633847953806</v>
       </c>
       <c r="G313" s="6"/>
@@ -17835,7 +17832,7 @@
         <v>33900</v>
       </c>
       <c r="F314">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86244180425878347</v>
       </c>
       <c r="G314" s="6"/>
@@ -17866,7 +17863,7 @@
         <v>36660</v>
       </c>
       <c r="F315">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.93282442748091599</v>
       </c>
       <c r="G315" s="6"/>
@@ -17897,7 +17894,7 @@
         <v>34620</v>
       </c>
       <c r="F316">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88120752411739256</v>
       </c>
       <c r="G316" s="6"/>
@@ -17928,7 +17925,7 @@
         <v>35370</v>
       </c>
       <c r="F317">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90043532496626866</v>
       </c>
       <c r="G317" s="6"/>
@@ -17959,7 +17956,7 @@
         <v>33630</v>
       </c>
       <c r="F318">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85637891520244458</v>
       </c>
       <c r="G318" s="6"/>
@@ -17990,7 +17987,7 @@
         <v>36000</v>
       </c>
       <c r="F319">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91698718765123921</v>
       </c>
       <c r="G319" s="6"/>
@@ -18021,7 +18018,7 @@
         <v>36180</v>
       </c>
       <c r="F320">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.92180692501719785</v>
       </c>
       <c r="G320" s="6"/>
@@ -18052,7 +18049,7 @@
         <v>34650</v>
       </c>
       <c r="F321">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88298251872993216</v>
       </c>
       <c r="G321" s="6"/>
@@ -18083,7 +18080,7 @@
         <v>33090</v>
       </c>
       <c r="F322">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.84340113167150943</v>
       </c>
       <c r="G322" s="6"/>
@@ -18114,7 +18111,7 @@
         <v>35850</v>
       </c>
       <c r="F323">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91391133657939683</v>
       </c>
       <c r="G323" s="6"/>
@@ -18145,7 +18142,7 @@
         <v>36000</v>
       </c>
       <c r="F324">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91782882492415163</v>
       </c>
       <c r="G324" s="6"/>
@@ -18176,7 +18173,7 @@
         <v>34650</v>
       </c>
       <c r="F325">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88370313695485847</v>
       </c>
       <c r="G325" s="6"/>
@@ -18207,7 +18204,7 @@
         <v>33960</v>
       </c>
       <c r="F326">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86645915191100675</v>
       </c>
       <c r="G326" s="6"/>
@@ -18238,7 +18235,7 @@
         <v>33990</v>
       </c>
       <c r="F327">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86737948809554188</v>
       </c>
       <c r="G327" s="6"/>
@@ -18269,7 +18266,7 @@
         <v>34380</v>
       </c>
       <c r="F328">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87757810904635492</v>
       </c>
       <c r="G328" s="6"/>
@@ -18300,7 +18297,7 @@
         <v>33510</v>
       </c>
       <c r="F329">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85547981925403993</v>
       </c>
       <c r="G329" s="6"/>
@@ -18331,7 +18328,7 @@
         <v>33690</v>
       </c>
       <c r="F330">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86031664964249233</v>
       </c>
       <c r="G330" s="6"/>
@@ -18362,7 +18359,7 @@
         <v>34290</v>
       </c>
       <c r="F331">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87577259028451759</v>
       </c>
       <c r="G331" s="6"/>
@@ -18393,7 +18390,7 @@
         <v>34320</v>
       </c>
       <c r="F332">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87687472853164361</v>
       </c>
       <c r="G332" s="6"/>
@@ -18424,7 +18421,7 @@
         <v>35310</v>
       </c>
       <c r="F333">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90235363266975033</v>
       </c>
       <c r="G333" s="6"/>
@@ -18455,7 +18452,7 @@
         <v>31350</v>
       </c>
       <c r="F334">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80140085380505632</v>
       </c>
       <c r="G334" s="6"/>
@@ -18486,7 +18483,7 @@
         <v>34080</v>
       </c>
       <c r="F335">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87141067273517603</v>
       </c>
       <c r="G335" s="6"/>
@@ -18517,7 +18514,7 @@
         <v>32160</v>
       </c>
       <c r="F336">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82261158715948335</v>
       </c>
       <c r="G336" s="6"/>
@@ -18548,7 +18545,7 @@
         <v>32700</v>
       </c>
       <c r="F337">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.83661669139845474</v>
       </c>
       <c r="G337" s="6"/>
@@ -18579,7 +18576,7 @@
         <v>32370</v>
       </c>
       <c r="F338">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82836451109348208</v>
       </c>
       <c r="G338" s="6"/>
@@ -18610,7 +18607,7 @@
         <v>35010</v>
       </c>
       <c r="F339">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.89624452807004074</v>
       </c>
       <c r="G339" s="6"/>
@@ -18641,7 +18638,7 @@
         <v>34740</v>
       </c>
       <c r="F340">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.88951478683907315</v>
       </c>
       <c r="G340" s="6"/>
@@ -18672,7 +18669,7 @@
         <v>28350</v>
       </c>
       <c r="F341">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72615967828692918</v>
       </c>
       <c r="G341" s="6"/>
@@ -18703,7 +18700,7 @@
         <v>34320</v>
       </c>
       <c r="F342">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87927854068456646</v>
       </c>
       <c r="G342" s="6"/>
@@ -18734,7 +18731,7 @@
         <v>33540</v>
       </c>
       <c r="F343">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85944907110826396</v>
       </c>
       <c r="G343" s="6"/>
@@ -18765,7 +18762,7 @@
         <v>35130</v>
       </c>
       <c r="F344">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90049215625961243</v>
       </c>
       <c r="G344" s="6"/>
@@ -18796,7 +18793,7 @@
         <v>32070</v>
       </c>
       <c r="F345">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8222655248448798</v>
       </c>
       <c r="G345" s="6"/>
@@ -18827,7 +18824,7 @@
         <v>35520</v>
       </c>
       <c r="F346">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.91102618687322068</v>
       </c>
       <c r="G346" s="6"/>
@@ -18858,7 +18855,7 @@
         <v>32520</v>
       </c>
       <c r="F347">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.83425258459249374</v>
       </c>
       <c r="G347" s="6"/>
@@ -18889,7 +18886,7 @@
         <v>33360</v>
       </c>
       <c r="F348">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85599917889767008</v>
       </c>
       <c r="G348" s="6"/>
@@ -18920,7 +18917,7 @@
         <v>34140</v>
       </c>
       <c r="F349">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.87632835361158168</v>
       </c>
       <c r="G349" s="6"/>
@@ -18951,7 +18948,7 @@
         <v>33900</v>
       </c>
       <c r="F350">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8704359882914805</v>
       </c>
       <c r="G350" s="6"/>
@@ -18982,7 +18979,7 @@
         <v>33240</v>
       </c>
       <c r="F351">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85364287732093791</v>
       </c>
       <c r="G351" s="6"/>
@@ -19013,7 +19010,7 @@
         <v>31620</v>
       </c>
       <c r="F352">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81233140655105973</v>
       </c>
       <c r="G352" s="6"/>
@@ -19044,7 +19041,7 @@
         <v>30240</v>
       </c>
       <c r="F353">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.77719807756560177</v>
       </c>
       <c r="G353" s="6"/>
@@ -19075,7 +19072,7 @@
         <v>33510</v>
       </c>
       <c r="F354">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.86152817770464829</v>
       </c>
       <c r="G354" s="6"/>
@@ -19106,7 +19103,7 @@
         <v>33060</v>
       </c>
       <c r="F355">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85024303680271585</v>
       </c>
       <c r="G355" s="6"/>
@@ -19137,7 +19134,7 @@
         <v>34410</v>
       </c>
       <c r="F356">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8851446945337621</v>
       </c>
       <c r="G356" s="6"/>
@@ -19168,7 +19165,7 @@
         <v>29940</v>
       </c>
       <c r="F357">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.77039857962586522</v>
       </c>
       <c r="G357" s="6"/>
@@ -19199,7 +19196,7 @@
         <v>30780</v>
       </c>
       <c r="F358">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7921556516368129</v>
       </c>
       <c r="G358" s="6"/>
@@ -19230,7 +19227,7 @@
         <v>32190</v>
       </c>
       <c r="F359">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82859275657031073</v>
       </c>
       <c r="G359" s="6"/>
@@ -19261,7 +19258,7 @@
         <v>31710</v>
       </c>
       <c r="F360">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81644738536007622</v>
       </c>
       <c r="G360" s="6"/>
@@ -19292,7 +19289,7 @@
         <v>31740</v>
       </c>
       <c r="F361">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81740921967550861</v>
       </c>
       <c r="G361" s="6"/>
@@ -19323,7 +19320,7 @@
         <v>30690</v>
       </c>
       <c r="F362">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7905718701700154</v>
       </c>
       <c r="G362" s="6"/>
@@ -19354,7 +19351,7 @@
         <v>30480</v>
       </c>
       <c r="F363">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78532412655879624</v>
       </c>
       <c r="G363" s="6"/>
@@ -19385,7 +19382,7 @@
         <v>29850</v>
       </c>
       <c r="F364">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76925059272239971</v>
       </c>
       <c r="G364" s="6"/>
@@ -19416,7 +19413,7 @@
         <v>28650</v>
       </c>
       <c r="F365">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7384781936282091</v>
       </c>
       <c r="G365" s="6"/>
@@ -19447,7 +19444,7 @@
         <v>28740</v>
       </c>
       <c r="F366">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74095080952872028</v>
       </c>
       <c r="G366" s="6"/>
@@ -19478,7 +19475,7 @@
         <v>29560</v>
       </c>
       <c r="F367">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76226823796384646</v>
       </c>
       <c r="G367" s="6"/>
@@ -19509,7 +19506,7 @@
         <v>28430</v>
       </c>
       <c r="F368">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73324220462693113</v>
       </c>
       <c r="G368" s="6"/>
@@ -19540,7 +19537,7 @@
         <v>33270</v>
       </c>
       <c r="F369">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85831484443527162</v>
       </c>
       <c r="G369" s="6"/>
@@ -19571,7 +19568,7 @@
         <v>28290</v>
       </c>
       <c r="F370">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72998916240904166</v>
       </c>
       <c r="G370" s="6"/>
@@ -19602,7 +19599,7 @@
         <v>35040</v>
       </c>
       <c r="F371">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.90437475803329459</v>
       </c>
       <c r="G371" s="6"/>
@@ -19633,7 +19630,7 @@
         <v>30750</v>
       </c>
       <c r="F372">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79381469912486768</v>
       </c>
       <c r="G372" s="6"/>
@@ -19664,7 +19661,7 @@
         <v>30720</v>
       </c>
       <c r="F373">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79324502285227361</v>
       </c>
       <c r="G373" s="6"/>
@@ -19695,7 +19692,7 @@
         <v>30240</v>
       </c>
       <c r="F374">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78101190629923289</v>
       </c>
       <c r="G374" s="6"/>
@@ -19726,7 +19723,7 @@
         <v>31410</v>
       </c>
       <c r="F375">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81141823818134851</v>
       </c>
       <c r="G375" s="6"/>
@@ -19757,7 +19754,7 @@
         <v>29520</v>
       </c>
       <c r="F376">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7627315711960313</v>
       </c>
       <c r="G376" s="6"/>
@@ -19788,7 +19785,7 @@
         <v>30270</v>
       </c>
       <c r="F377">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78223118071168307</v>
       </c>
       <c r="G377" s="6"/>
@@ -19819,7 +19816,7 @@
         <v>29430</v>
       </c>
       <c r="F378">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76062235087356556</v>
       </c>
       <c r="G378" s="6"/>
@@ -19850,7 +19847,7 @@
         <v>30060</v>
       </c>
       <c r="F379">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7770654534174336</v>
       </c>
       <c r="G379" s="6"/>
@@ -19881,7 +19878,7 @@
         <v>30570</v>
       </c>
       <c r="F380">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79037178757950255</v>
       </c>
       <c r="G380" s="6"/>
@@ -19912,7 +19909,7 @@
         <v>29070</v>
       </c>
       <c r="F381">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7518621973929237</v>
       </c>
       <c r="G381" s="6"/>
@@ -19943,7 +19940,7 @@
         <v>29400</v>
       </c>
       <c r="F382">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7604956155099718</v>
       </c>
       <c r="G382" s="6"/>
@@ -19974,7 +19971,7 @@
         <v>28380</v>
       </c>
       <c r="F383">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73428201811125482</v>
       </c>
       <c r="G383" s="6"/>
@@ -20005,7 +20002,7 @@
         <v>29990</v>
       </c>
       <c r="F384">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.77605837904978781</v>
       </c>
       <c r="G384" s="6"/>
@@ -20036,7 +20033,7 @@
         <v>27810</v>
       </c>
       <c r="F385">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71981364048142871</v>
       </c>
       <c r="G385" s="6"/>
@@ -20067,7 +20064,7 @@
         <v>29430</v>
       </c>
       <c r="F386">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76188257222739986</v>
       </c>
       <c r="G386" s="6"/>
@@ -20098,7 +20095,7 @@
         <v>29580</v>
       </c>
       <c r="F387">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76614260923618849</v>
       </c>
       <c r="G387" s="6"/>
@@ -20129,7 +20126,7 @@
         <v>29340</v>
       </c>
       <c r="F388">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76012331925697552</v>
       </c>
       <c r="G388" s="6"/>
@@ -20160,7 +20157,7 @@
         <v>30200</v>
       </c>
       <c r="F389">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78262672333367889</v>
       </c>
       <c r="G389" s="6"/>
@@ -20191,7 +20188,7 @@
         <v>28980</v>
       </c>
       <c r="F390">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75120535019959567</v>
       </c>
       <c r="G390" s="6"/>
@@ -20222,7 +20219,7 @@
         <v>24710</v>
       </c>
       <c r="F391">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.64062013896090431</v>
       </c>
       <c r="G391" s="6"/>
@@ -20253,7 +20250,7 @@
         <v>33940</v>
       </c>
       <c r="F392">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8801410715211867</v>
       </c>
       <c r="G392" s="6"/>
@@ -20284,7 +20281,7 @@
         <v>27100</v>
       </c>
       <c r="F393">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70292843617876688</v>
       </c>
       <c r="G393" s="6"/>
@@ -20315,7 +20312,7 @@
         <v>30710</v>
       </c>
       <c r="F394">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7967310935270463</v>
       </c>
       <c r="G394" s="6"/>
@@ -20346,7 +20343,7 @@
         <v>29130</v>
       </c>
       <c r="F395">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75593616193071234</v>
       </c>
       <c r="G395" s="6"/>
@@ -20377,7 +20374,7 @@
         <v>28890</v>
       </c>
       <c r="F396">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74986373192825806</v>
       </c>
       <c r="G396" s="6"/>
@@ -20408,7 +20405,7 @@
         <v>28650</v>
       </c>
       <c r="F397">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74382740088791965</v>
       </c>
       <c r="G397" s="6"/>
@@ -20439,7 +20436,7 @@
         <v>28290</v>
       </c>
       <c r="F398">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73470977795091541</v>
       </c>
       <c r="G398" s="6"/>
@@ -20470,7 +20467,7 @@
         <v>29580</v>
       </c>
       <c r="F399">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76831168831168828</v>
       </c>
       <c r="G399" s="6"/>
@@ -20501,7 +20498,7 @@
         <v>27810</v>
       </c>
       <c r="F400">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72248778967058092</v>
       </c>
       <c r="G400" s="6"/>
@@ -20532,7 +20529,7 @@
         <v>28650</v>
       </c>
       <c r="F401">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74456196886613479</v>
       </c>
       <c r="G401" s="6"/>
@@ -20563,7 +20560,7 @@
         <v>27600</v>
       </c>
       <c r="F402">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71742351381560132</v>
       </c>
       <c r="G402" s="6"/>
@@ -20594,7 +20591,7 @@
         <v>28050</v>
       </c>
       <c r="F403">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72929124850501792</v>
       </c>
       <c r="G403" s="6"/>
@@ -20625,7 +20622,7 @@
         <v>27300</v>
       </c>
       <c r="F404">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70990222592053254</v>
       </c>
       <c r="G404" s="6"/>
@@ -20656,7 +20653,7 @@
         <v>26010</v>
       </c>
       <c r="F405">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.67644534602481077</v>
       </c>
       <c r="G405" s="6"/>
@@ -20687,7 +20684,7 @@
         <v>28140</v>
       </c>
       <c r="F406">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73210708431979599</v>
       </c>
       <c r="G406" s="6"/>
@@ -20718,7 +20715,7 @@
         <v>27330</v>
       </c>
       <c r="F407">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71114464885118789</v>
       </c>
       <c r="G407" s="6"/>
@@ -20749,7 +20746,7 @@
         <v>27720</v>
       </c>
       <c r="F408">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72146166258914168</v>
       </c>
       <c r="G408" s="6"/>
@@ -20780,7 +20777,7 @@
         <v>28950</v>
       </c>
       <c r="F409">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75365110769791477</v>
       </c>
       <c r="G409" s="6"/>
@@ -20811,7 +20808,7 @@
         <v>27240</v>
       </c>
       <c r="F410">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70922724432409912</v>
       </c>
       <c r="G410" s="6"/>
@@ -20842,7 +20839,7 @@
         <v>28080</v>
       </c>
       <c r="F411">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73119287555659718</v>
       </c>
       <c r="G411" s="6"/>
@@ -20873,7 +20870,7 @@
         <v>26550</v>
       </c>
       <c r="F412">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.69144226261784469</v>
       </c>
       <c r="G412" s="6"/>
@@ -20904,7 +20901,7 @@
         <v>25560</v>
       </c>
       <c r="F413">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.66572902015939994</v>
       </c>
       <c r="G413" s="6"/>
@@ -20935,7 +20932,7 @@
         <v>24630</v>
       </c>
       <c r="F414">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.64160675211003437</v>
       </c>
       <c r="G414" s="6"/>
@@ -20966,7 +20963,7 @@
         <v>26700</v>
       </c>
       <c r="F415">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.69560233430596086</v>
       </c>
       <c r="G415" s="6"/>
@@ -20997,7 +20994,7 @@
         <v>25800</v>
       </c>
       <c r="F416">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.67224263268975226</v>
       </c>
       <c r="G416" s="6"/>
@@ -21028,7 +21025,7 @@
         <v>25560</v>
       </c>
       <c r="F417">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.66609334688452815</v>
       </c>
       <c r="G417" s="6"/>
@@ -21059,7 +21056,7 @@
         <v>25920</v>
       </c>
       <c r="F418">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.67556296914095082</v>
       </c>
       <c r="G418" s="6"/>
@@ -21090,7 +21087,7 @@
         <v>31830</v>
       </c>
       <c r="F419">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82972733434127521</v>
       </c>
       <c r="G419" s="6"/>
@@ -21121,7 +21118,7 @@
         <v>23460</v>
       </c>
       <c r="F420">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.61162238965508253</v>
       </c>
       <c r="G420" s="6"/>
@@ -21152,7 +21149,7 @@
         <v>27870</v>
       </c>
       <c r="F421">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7266896120150188</v>
       </c>
       <c r="G421" s="6"/>
@@ -21183,7 +21180,7 @@
         <v>26920</v>
       </c>
       <c r="F422">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7020288947999791</v>
       </c>
       <c r="G422" s="6"/>
@@ -21214,7 +21211,7 @@
         <v>28410</v>
       </c>
       <c r="F423">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74096291273277348</v>
       </c>
       <c r="G423" s="6"/>
@@ -21245,7 +21242,7 @@
         <v>27630</v>
       </c>
       <c r="F424">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72069487192863479</v>
       </c>
       <c r="G424" s="6"/>
@@ -21276,7 +21273,7 @@
         <v>30240</v>
       </c>
       <c r="F425">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78885584598528724</v>
       </c>
       <c r="G425" s="6"/>
@@ -21307,7 +21304,7 @@
         <v>25740</v>
       </c>
       <c r="F426">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.6715892190883711</v>
       </c>
       <c r="G426" s="6"/>
@@ -21338,7 +21335,7 @@
         <v>27120</v>
       </c>
       <c r="F427">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70768749021449817</v>
       </c>
       <c r="G427" s="6"/>
@@ -21369,7 +21366,7 @@
         <v>30540</v>
       </c>
       <c r="F428">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79701445795709591</v>
       </c>
       <c r="G428" s="6"/>
@@ -21400,7 +21397,7 @@
         <v>26820</v>
       </c>
       <c r="F429">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7000234907211651</v>
       </c>
       <c r="G429" s="6"/>
@@ -21431,7 +21428,7 @@
         <v>29100</v>
       </c>
       <c r="F430">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75965228287258202</v>
       </c>
       <c r="G430" s="6"/>
@@ -21462,7 +21459,7 @@
         <v>28950</v>
       </c>
       <c r="F431">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75587467362924277</v>
       </c>
       <c r="G431" s="6"/>
@@ -21493,7 +21490,7 @@
         <v>28800</v>
       </c>
       <c r="F432">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75207604324437249</v>
       </c>
       <c r="G432" s="6"/>
@@ -21524,7 +21521,7 @@
         <v>29190</v>
       </c>
       <c r="F433">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76239977015697236</v>
       </c>
       <c r="G433" s="6"/>
@@ -21555,7 +21552,7 @@
         <v>30840</v>
       </c>
       <c r="F434">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80560054333629383</v>
       </c>
       <c r="G434" s="6"/>
@@ -21586,7 +21583,7 @@
         <v>29910</v>
       </c>
       <c r="F435">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78147044991377956</v>
       </c>
       <c r="G435" s="6"/>
@@ -21617,7 +21614,7 @@
         <v>30710</v>
       </c>
       <c r="F436">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80247720086754293</v>
       </c>
       <c r="G436" s="6"/>
@@ -21648,7 +21645,7 @@
         <v>32640</v>
       </c>
       <c r="F437">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.8529988239905919</v>
       </c>
       <c r="G437" s="6"/>
@@ -21679,7 +21676,7 @@
         <v>29730</v>
       </c>
       <c r="F438">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.77703144193826612</v>
       </c>
       <c r="G438" s="6"/>
@@ -21710,7 +21707,7 @@
         <v>30480</v>
       </c>
       <c r="F439">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79673776662484319</v>
       </c>
       <c r="G439" s="6"/>
@@ -21741,7 +21738,7 @@
         <v>30660</v>
       </c>
       <c r="F440">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80156862745098034</v>
       </c>
       <c r="G440" s="6"/>
@@ -21772,7 +21769,7 @@
         <v>31620</v>
       </c>
       <c r="F441">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82679636021336678</v>
       </c>
       <c r="G441" s="6"/>
@@ -21803,7 +21800,7 @@
         <v>29160</v>
       </c>
       <c r="F442">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7625921857837753</v>
       </c>
       <c r="G442" s="6"/>
@@ -21834,7 +21831,7 @@
         <v>28080</v>
       </c>
       <c r="F443">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7344632768361582</v>
       </c>
       <c r="G443" s="6"/>
@@ -21865,7 +21862,7 @@
         <v>32340</v>
       </c>
       <c r="F444">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.84608743426732591</v>
       </c>
       <c r="G444" s="6"/>
@@ -21896,7 +21893,7 @@
         <v>29160</v>
       </c>
       <c r="F445">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76299126066251499</v>
       </c>
       <c r="G445" s="6"/>
@@ -21927,7 +21924,7 @@
         <v>30330</v>
       </c>
       <c r="F446">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79368817710786621</v>
       </c>
       <c r="G446" s="6"/>
@@ -21958,7 +21955,7 @@
         <v>31050</v>
       </c>
       <c r="F447">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81261449882229786</v>
       </c>
       <c r="G447" s="6"/>
@@ -21989,7 +21986,7 @@
         <v>31470</v>
       </c>
       <c r="F448">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82373573447806514</v>
       </c>
       <c r="G448" s="6"/>
@@ -22020,7 +22017,7 @@
         <v>30480</v>
       </c>
       <c r="F449">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79794753652023664</v>
       </c>
       <c r="G449" s="6"/>
@@ -22051,7 +22048,7 @@
         <v>30660</v>
       </c>
       <c r="F450">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80278592375366564</v>
       </c>
       <c r="G450" s="6"/>
@@ -22082,7 +22079,7 @@
         <v>29400</v>
       </c>
       <c r="F451">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76991567590216314</v>
       </c>
       <c r="G451" s="6"/>
@@ -22113,7 +22110,7 @@
         <v>32730</v>
       </c>
       <c r="F452">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85725510738606603</v>
       </c>
       <c r="G452" s="6"/>
@@ -22144,7 +22141,7 @@
         <v>30690</v>
       </c>
       <c r="F453">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80392927308447937</v>
       </c>
       <c r="G453" s="6"/>
@@ -22175,7 +22172,7 @@
         <v>30840</v>
       </c>
       <c r="F454">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80794320295512301</v>
       </c>
       <c r="G454" s="6"/>
@@ -22206,7 +22203,7 @@
         <v>30780</v>
       </c>
       <c r="F455">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80647696903002675</v>
       </c>
       <c r="G455" s="6"/>
@@ -22237,7 +22234,7 @@
         <v>29820</v>
       </c>
       <c r="F456">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78146701957598474</v>
       </c>
       <c r="G456" s="6"/>
@@ -22268,7 +22265,7 @@
         <v>31770</v>
       </c>
       <c r="F457">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.83276539973787678</v>
       </c>
       <c r="G457" s="6"/>
@@ -22299,7 +22296,7 @@
         <v>30600</v>
       </c>
       <c r="F458">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.80220212347620923</v>
       </c>
       <c r="G458" s="6"/>
@@ -22330,7 +22327,7 @@
         <v>31230</v>
       </c>
       <c r="F459">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.81880391180094914</v>
       </c>
       <c r="G459" s="6"/>
@@ -22361,7 +22358,7 @@
         <v>29250</v>
       </c>
       <c r="F460">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7669918187539333</v>
       </c>
       <c r="G460" s="6"/>
@@ -22392,7 +22389,7 @@
         <v>32490</v>
       </c>
       <c r="F461">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85206262620964568</v>
       </c>
       <c r="G461" s="6"/>
@@ -22423,7 +22420,7 @@
         <v>27420</v>
       </c>
       <c r="F462">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71917538752065469</v>
       </c>
       <c r="G462" s="6"/>
@@ -22454,7 +22451,7 @@
         <v>32160</v>
       </c>
       <c r="F463">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.84362949555363187</v>
       </c>
       <c r="G463" s="6"/>
@@ -22485,7 +22482,7 @@
         <v>28980</v>
       </c>
       <c r="F464">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76033057851239672</v>
       </c>
       <c r="G464" s="6"/>
@@ -22516,7 +22513,7 @@
         <v>29940</v>
       </c>
       <c r="F465">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78559995801737026</v>
       </c>
       <c r="G465" s="6"/>
@@ -22547,7 +22544,7 @@
         <v>29160</v>
       </c>
       <c r="F466">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76523382144544161</v>
       </c>
       <c r="G466" s="6"/>
@@ -22578,7 +22575,7 @@
         <v>28650</v>
       </c>
       <c r="F467">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75198824116118534</v>
       </c>
       <c r="G467" s="6"/>
@@ -22609,7 +22606,7 @@
         <v>28740</v>
       </c>
       <c r="F468">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75442971518571988</v>
       </c>
       <c r="G468" s="6"/>
@@ -22640,7 +22637,7 @@
         <v>30030</v>
       </c>
       <c r="F469">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.78839590443686003</v>
       </c>
       <c r="G469" s="6"/>
@@ -22671,7 +22668,7 @@
         <v>31230</v>
       </c>
       <c r="F470">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.82002940867555929</v>
       </c>
       <c r="G470" s="6"/>
@@ -22702,7 +22699,7 @@
         <v>27840</v>
       </c>
       <c r="F471">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7311500380807312</v>
       </c>
       <c r="G471" s="6"/>
@@ -22733,7 +22730,7 @@
         <v>32460</v>
       </c>
       <c r="F472">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.85259508300063036</v>
       </c>
       <c r="G472" s="6"/>
@@ -22764,7 +22761,7 @@
         <v>22800</v>
       </c>
       <c r="F473">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.59895970157095568</v>
       </c>
       <c r="G473" s="6"/>
@@ -22795,7 +22792,7 @@
         <v>28350</v>
       </c>
       <c r="F474">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74489608239838145</v>
       </c>
       <c r="G474" s="6"/>
@@ -22826,7 +22823,7 @@
         <v>29130</v>
       </c>
       <c r="F475">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76551126061020158</v>
       </c>
       <c r="G475" s="6"/>
@@ -22857,7 +22854,7 @@
         <v>26880</v>
       </c>
       <c r="F476">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.706513168269989</v>
       </c>
       <c r="G476" s="6"/>
@@ -22888,7 +22885,7 @@
         <v>28140</v>
       </c>
       <c r="F477">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73974763406940058</v>
       </c>
       <c r="G477" s="6"/>
@@ -22919,7 +22916,7 @@
         <v>28170</v>
       </c>
       <c r="F478">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74065309985802175</v>
       </c>
       <c r="G478" s="6"/>
@@ -22950,7 +22947,7 @@
         <v>26700</v>
       </c>
       <c r="F479">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70211423161880715</v>
       </c>
       <c r="G479" s="6"/>
@@ -22981,7 +22978,7 @@
         <v>27150</v>
       </c>
       <c r="F480">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71409784324039982</v>
       </c>
       <c r="G480" s="6"/>
@@ -23012,7 +23009,7 @@
         <v>28290</v>
       </c>
       <c r="F481">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74421908294530814</v>
       </c>
       <c r="G481" s="6"/>
@@ -23043,7 +23040,7 @@
         <v>28830</v>
       </c>
       <c r="F482">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.75856443719412725</v>
       </c>
       <c r="G482" s="6"/>
@@ -23074,7 +23071,7 @@
         <v>27300</v>
       </c>
       <c r="F483">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71845886625611877</v>
       </c>
       <c r="G483" s="6"/>
@@ -23105,7 +23102,7 @@
         <v>26880</v>
       </c>
       <c r="F484">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70757324488667772</v>
       </c>
       <c r="G484" s="6"/>
@@ -23136,7 +23133,7 @@
         <v>27270</v>
       </c>
       <c r="F485">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71797167079142754</v>
       </c>
       <c r="G485" s="6"/>
@@ -23167,7 +23164,7 @@
         <v>28920</v>
       </c>
       <c r="F486">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76151354767359192</v>
       </c>
       <c r="G486" s="6"/>
@@ -23198,7 +23195,7 @@
         <v>27090</v>
       </c>
       <c r="F487">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71343920360274948</v>
       </c>
       <c r="G487" s="6"/>
@@ -23229,7 +23226,7 @@
         <v>29130</v>
       </c>
       <c r="F488">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.76732608065748231</v>
       </c>
       <c r="G488" s="6"/>
@@ -23260,7 +23257,7 @@
         <v>27540</v>
       </c>
       <c r="F489">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.72551963961115939</v>
       </c>
       <c r="G489" s="6"/>
@@ -23291,7 +23288,7 @@
         <v>25980</v>
       </c>
       <c r="F490">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.68451283132212681</v>
       </c>
       <c r="G490" s="6"/>
@@ -23322,7 +23319,7 @@
         <v>28400</v>
       </c>
       <c r="F491">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74839253715610832</v>
       </c>
       <c r="G491" s="6"/>
@@ -23353,7 +23350,7 @@
         <v>30350</v>
       </c>
       <c r="F492">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.79992620120713742</v>
       </c>
       <c r="G492" s="6"/>
@@ -23384,7 +23381,7 @@
         <v>28680</v>
       </c>
       <c r="F493">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7560699127408852</v>
       </c>
       <c r="G493" s="6"/>
@@ -23415,7 +23412,7 @@
         <v>28160</v>
       </c>
       <c r="F494">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74251812788398153</v>
       </c>
       <c r="G494" s="6"/>
@@ -23446,7 +23443,7 @@
         <v>27960</v>
       </c>
       <c r="F495">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.73734177215189878</v>
       </c>
       <c r="G495" s="6"/>
@@ -23477,7 +23474,7 @@
         <v>26580</v>
       </c>
       <c r="F496">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70106029435037187</v>
       </c>
       <c r="G496" s="6"/>
@@ -23508,7 +23505,7 @@
         <v>26520</v>
       </c>
       <c r="F497">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.69964384645825084</v>
       </c>
       <c r="G497" s="6"/>
@@ -23539,7 +23536,7 @@
         <v>26280</v>
       </c>
       <c r="F498">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.69342199002612204</v>
       </c>
       <c r="G498" s="6"/>
@@ -23570,7 +23567,7 @@
         <v>26760</v>
       </c>
       <c r="F499">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.70623630941384496</v>
       </c>
       <c r="G499" s="6"/>
@@ -23601,7 +23598,7 @@
         <v>29190</v>
       </c>
       <c r="F500">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.77046930264477642</v>
       </c>
       <c r="G500" s="6"/>
@@ -23632,7 +23629,7 @@
         <v>25980</v>
       </c>
       <c r="F501">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.68597681725767701</v>
       </c>
       <c r="G501" s="6"/>
@@ -23663,7 +23660,7 @@
         <v>26340</v>
       </c>
       <c r="F502">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.69573945429092154</v>
       </c>
       <c r="G502" s="6"/>
@@ -23694,7 +23691,7 @@
         <v>28080</v>
       </c>
       <c r="F503">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.74187582562747689</v>
       </c>
       <c r="G503" s="6"/>
@@ -23725,7 +23722,7 @@
         <v>24000</v>
       </c>
       <c r="F504">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.6342662332514073</v>
       </c>
       <c r="G504" s="6"/>
@@ -23756,7 +23753,7 @@
         <v>27000</v>
       </c>
       <c r="F505">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.7136626754420744</v>
       </c>
       <c r="G505" s="6"/>
@@ -23787,7 +23784,7 @@
         <v>26980</v>
       </c>
       <c r="F506">
-        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[42139]]</f>
+        <f>CicloZ[[#This Row],[Eggs]]/CicloZ[[#This Row],[Chickens]]</f>
         <v>0.71322829649994712</v>
       </c>
       <c r="G506" s="6"/>
@@ -31772,7 +31769,7 @@
       </c>
       <c r="G215" s="6">
         <f ca="1">RANDBETWEEN(158, 170)</f>
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H215" s="6">
         <v>123</v>
@@ -31810,7 +31807,7 @@
       </c>
       <c r="G216" s="6">
         <f t="shared" ref="G216:G234" ca="1" si="0">RANDBETWEEN(158, 170)</f>
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="H216" s="6">
         <v>132</v>
@@ -31848,7 +31845,7 @@
       </c>
       <c r="G217" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H217" s="6">
         <v>129.5</v>
@@ -31886,7 +31883,7 @@
       </c>
       <c r="G218" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="H218" s="6">
         <v>135.5</v>
@@ -31924,7 +31921,7 @@
       </c>
       <c r="G219" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="H219" s="6">
         <v>119</v>
@@ -31962,7 +31959,7 @@
       </c>
       <c r="G220" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="H220" s="6">
         <v>111</v>
@@ -32000,7 +31997,7 @@
       </c>
       <c r="G221" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H221" s="6">
         <v>129.5</v>
@@ -32038,7 +32035,7 @@
       </c>
       <c r="G222" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H222" s="6">
         <v>117.5</v>
@@ -32076,7 +32073,7 @@
       </c>
       <c r="G223" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H223" s="6">
         <v>115</v>
@@ -32114,7 +32111,7 @@
       </c>
       <c r="G224" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H224" s="6">
         <v>126.5</v>
@@ -32190,7 +32187,7 @@
       </c>
       <c r="G226" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H226" s="6">
         <v>132.5</v>
@@ -32228,7 +32225,7 @@
       </c>
       <c r="G227" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H227" s="6">
         <v>127.5</v>
@@ -32266,7 +32263,7 @@
       </c>
       <c r="G228" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H228" s="6">
         <v>116</v>
@@ -32304,7 +32301,7 @@
       </c>
       <c r="G229" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H229" s="6">
         <v>108</v>
@@ -32342,7 +32339,7 @@
       </c>
       <c r="G230" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H230" s="6">
         <v>130</v>
@@ -32380,7 +32377,7 @@
       </c>
       <c r="G231" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="H231" s="6">
         <v>118.5</v>
@@ -32418,7 +32415,7 @@
       </c>
       <c r="G232" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="H232" s="6">
         <v>126</v>
@@ -32456,7 +32453,7 @@
       </c>
       <c r="G233" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H233" s="6">
         <v>126</v>
@@ -32494,7 +32491,7 @@
       </c>
       <c r="G234" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H234" s="6">
         <v>130.5</v>

</xml_diff>